<commit_message>
Finishing up, adding enums
</commit_message>
<xml_diff>
--- a/Documentation/TestCases.xlsx
+++ b/Documentation/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bhawana\Food Recommendation System\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F14B23F-02BC-4422-987C-05D94E436CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71EAF50-F872-4787-AEE0-A36AFED5A9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2850" windowWidth="29040" windowHeight="15840" xr2:uid="{24442B6E-26B0-481E-933F-86C178DA3CF7}"/>
+    <workbookView xWindow="7665" yWindow="1545" windowWidth="15375" windowHeight="7875" xr2:uid="{24442B6E-26B0-481E-933F-86C178DA3CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t xml:space="preserve">Test Case ID </t>
   </si>
@@ -68,9 +68,6 @@
     <t>Invalid email or password should not be allowed</t>
   </si>
   <si>
-    <t>{Dish name, price, description}</t>
-  </si>
-  <si>
     <t>{Dish name}</t>
   </si>
   <si>
@@ -138,6 +135,51 @@
   </si>
   <si>
     <t>Logging In</t>
+  </si>
+  <si>
+    <t>The Employee should be able to send review and rating for the food</t>
+  </si>
+  <si>
+    <t>{Dish name, type, cusine, diet-type, spice level}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{total rating, review text, quantity rating, quality rating, appearance rating, value for money rating, food id}</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Whenver choosing a meal Recommendation system should send a list of items</t>
+  </si>
+  <si>
+    <t>{classification, number of dishes}</t>
+  </si>
+  <si>
+    <t>Discard Menu Items</t>
+  </si>
+  <si>
+    <t>The chef should receive a list of dishes which have very low feedback and then gets one of these dishes</t>
+  </si>
+  <si>
+    <t>When Chef chooses to get feedback and employee sends a feedback the Chef should be able to decide the discard option twice</t>
+  </si>
+  <si>
+    <t>The chef should not take a dish if there are no dishes that match requirement</t>
+  </si>
+  <si>
+    <t>Sorting Profile</t>
+  </si>
+  <si>
+    <t>The dishes should be sorted according to the user profile and natural order</t>
+  </si>
+  <si>
+    <t>{userEmail}</t>
+  </si>
+  <si>
+    <t>If the user does not exist then no sorting should be done</t>
   </si>
 </sst>
 </file>
@@ -516,10 +558,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A734CF4E-9365-428F-A914-4A2F2B09708D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -557,12 +599,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -571,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
@@ -587,194 +629,308 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -804,6 +960,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="84d9b681-5f57-44f2-8788-7a46af99f0a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067DA1B12F002F34D87304BA97FDFCC4E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8c00a287bf5d8e0f20af3e60306acb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="84d9b681-5f57-44f2-8788-7a46af99f0a9" xmlns:ns4="d9dc719c-51f1-42ca-8c7d-85c14afb6451" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="256cc7d9099e8b1e7ba971015aa00ad1" ns3:_="" ns4:_="">
     <xsd:import namespace="84d9b681-5f57-44f2-8788-7a46af99f0a9"/>
@@ -1028,14 +1192,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="84d9b681-5f57-44f2-8788-7a46af99f0a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E34F4929-BF1D-41D7-8FC4-394C8F8A0AB7}">
   <ds:schemaRefs>
@@ -1045,6 +1201,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15DB622F-A1C7-4C90-9C82-B32B21A63442}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="84d9b681-5f57-44f2-8788-7a46af99f0a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d9dc719c-51f1-42ca-8c7d-85c14afb6451"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C11FE979-71E7-4C3D-89AB-4C554334391A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1061,21 +1234,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15DB622F-A1C7-4C90-9C82-B32B21A63442}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="84d9b681-5f57-44f2-8788-7a46af99f0a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d9dc719c-51f1-42ca-8c7d-85c14afb6451"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>